<commit_message>
Create Indent With & Without WO.
</commit_message>
<xml_diff>
--- a/IN4RE/ExecutionController/TestSet1.xlsx
+++ b/IN4RE/ExecutionController/TestSet1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20354"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919C412C-8328-4933-AE02-4DCC8FF5CD38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABE1F37-621D-42FB-9219-39DC08221048}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11265" windowHeight="2580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Status</t>
   </si>
@@ -515,7 +515,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +613,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D6" s="3"/>
     </row>
@@ -625,7 +625,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D7" s="3"/>
     </row>

</xml_diff>